<commit_message>
Test NavLinks in Header
</commit_message>
<xml_diff>
--- a/_site/raw_data/2021-02-12_TexasCOVID19Demographics.xlsx
+++ b/_site/raw_data/2021-02-12_TexasCOVID19Demographics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdavis197\Desktop\Leadership Reports\Demographics Thursday\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78CCCF93-41DA-44BE-89AA-DA3ADA48391A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5681616A-11B9-427C-8130-4A8EA86ABE01}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="806" xr2:uid="{A6E7ED99-6879-4496-BF23-313330724014}"/>
   </bookViews>
@@ -549,7 +549,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -573,11 +573,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C2" s="12">
         <f>B2/$B$15</f>
-        <v>3.6088507412774494E-3</v>
+        <v>3.5567864027585458E-3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -585,11 +585,11 @@
         <v>3</v>
       </c>
       <c r="B3" s="4">
-        <v>1242</v>
+        <v>1251</v>
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C15" si="0">B3/$B$15</f>
-        <v>1.7305763014156726E-2</v>
+        <v>1.6982976297140996E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -597,11 +597,11 @@
         <v>4</v>
       </c>
       <c r="B4" s="4">
-        <v>3328</v>
+        <v>3376</v>
       </c>
       <c r="C4" s="12">
         <f t="shared" si="0"/>
-        <v>4.6371641957418351E-2</v>
+        <v>4.5830957617224617E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -609,11 +609,11 @@
         <v>5</v>
       </c>
       <c r="B5" s="4">
-        <v>14267</v>
+        <v>14683</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" si="0"/>
-        <v>0.19879333407646863</v>
+        <v>0.19932936928131192</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -621,11 +621,11 @@
         <v>6</v>
       </c>
       <c r="B6" s="4">
-        <v>15704</v>
+        <v>16200</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" si="0"/>
-        <v>0.21881618548656784</v>
+        <v>0.21992343406369635</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -633,11 +633,11 @@
         <v>7</v>
       </c>
       <c r="B7" s="4">
-        <v>13740</v>
+        <v>14164</v>
       </c>
       <c r="C7" s="12">
         <f t="shared" si="0"/>
-        <v>0.19145022851410098</v>
+        <v>0.19228367407890093</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -645,11 +645,11 @@
         <v>8</v>
       </c>
       <c r="B8" s="4">
-        <v>11681</v>
+        <v>11971</v>
       </c>
       <c r="C8" s="12">
         <f t="shared" si="0"/>
-        <v>0.16276056181027757</v>
+        <v>0.16251255735657463</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -657,11 +657,11 @@
         <v>9</v>
       </c>
       <c r="B9" s="4">
-        <v>4221</v>
+        <v>4320</v>
       </c>
       <c r="C9" s="12">
         <f t="shared" si="0"/>
-        <v>5.8814513432170326E-2</v>
+        <v>5.864624908365236E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -669,11 +669,11 @@
         <v>10</v>
       </c>
       <c r="B10" s="4">
-        <v>2838</v>
+        <v>2888</v>
       </c>
       <c r="C10" s="12">
         <f t="shared" si="0"/>
-        <v>3.9544086500947498E-2</v>
+        <v>3.9206103554071302E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -681,11 +681,11 @@
         <v>11</v>
       </c>
       <c r="B11" s="4">
-        <v>1685</v>
+        <v>1714</v>
       </c>
       <c r="C11" s="12">
         <f t="shared" si="0"/>
-        <v>2.347843049827221E-2</v>
+        <v>2.3268442344763923E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -693,11 +693,11 @@
         <v>12</v>
       </c>
       <c r="B12" s="4">
-        <v>1089</v>
+        <v>1103</v>
       </c>
       <c r="C12" s="12">
         <f t="shared" si="0"/>
-        <v>1.5173893657340318E-2</v>
+        <v>1.4973799245201053E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -705,11 +705,11 @@
         <v>13</v>
       </c>
       <c r="B13" s="4">
-        <v>1700</v>
+        <v>1716</v>
       </c>
       <c r="C13" s="12">
         <f t="shared" si="0"/>
-        <v>2.3687437297960093E-2</v>
+        <v>2.3295593386006352E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -721,7 +721,7 @@
       </c>
       <c r="C14" s="12">
         <f t="shared" si="0"/>
-        <v>1.9507301304202431E-4</v>
+        <v>1.9005728869702154E-4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -730,7 +730,7 @@
       </c>
       <c r="B15" s="1">
         <f>SUM(B2:B14)</f>
-        <v>71768</v>
+        <v>73662</v>
       </c>
       <c r="C15" s="11">
         <f t="shared" si="0"/>
@@ -768,11 +768,11 @@
         <v>16</v>
       </c>
       <c r="B2" s="4">
-        <v>24344</v>
+        <v>24724</v>
       </c>
       <c r="C2" s="12">
         <f>B2/$B$5</f>
-        <v>0.33920410210678853</v>
+        <v>0.33564117183894004</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -780,11 +780,11 @@
         <v>17</v>
       </c>
       <c r="B3" s="4">
-        <v>46529</v>
+        <v>48028</v>
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C5" si="0">B3/$B$5</f>
-        <v>0.64832515884516773</v>
+        <v>0.65200510439575354</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -792,11 +792,11 @@
         <v>18</v>
       </c>
       <c r="B4" s="4">
-        <v>895</v>
+        <v>910</v>
       </c>
       <c r="C4" s="12">
         <f t="shared" si="0"/>
-        <v>1.2470739048043696E-2</v>
+        <v>1.23537237653064E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -805,7 +805,7 @@
       </c>
       <c r="B5" s="1">
         <f>SUM(B2:B4)</f>
-        <v>71768</v>
+        <v>73662</v>
       </c>
       <c r="C5" s="11">
         <f t="shared" si="0"/>
@@ -822,7 +822,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -846,11 +846,11 @@
         <v>23</v>
       </c>
       <c r="B2" s="4">
-        <v>922</v>
+        <v>928</v>
       </c>
       <c r="C2" s="12">
         <f>B2/$B$8</f>
-        <v>1.2846951287481886E-2</v>
+        <v>1.2598083136488284E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -858,11 +858,11 @@
         <v>21</v>
       </c>
       <c r="B3" s="4">
-        <v>12018</v>
+        <v>12369</v>
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C8" si="0">B3/$B$8</f>
-        <v>0.16745624790993199</v>
+        <v>0.16791561456381851</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -870,11 +870,11 @@
         <v>22</v>
       </c>
       <c r="B4" s="4">
-        <v>27129</v>
+        <v>27435</v>
       </c>
       <c r="C4" s="12">
         <f t="shared" si="0"/>
-        <v>0.37800969791550554</v>
+        <v>0.37244440824305614</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -882,11 +882,11 @@
         <v>25</v>
       </c>
       <c r="B5" s="4">
-        <v>385</v>
+        <v>400</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" si="0"/>
-        <v>5.3645078586556684E-3</v>
+        <v>5.4302082484863293E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -894,11 +894,11 @@
         <v>20</v>
       </c>
       <c r="B6" s="4">
-        <v>23170</v>
+        <v>24275</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" si="0"/>
-        <v>0.32284583658455024</v>
+        <v>0.3295457630800141</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -906,11 +906,11 @@
         <v>18</v>
       </c>
       <c r="B7" s="4">
-        <v>8144</v>
+        <v>8255</v>
       </c>
       <c r="C7" s="12">
         <f t="shared" si="0"/>
-        <v>0.11347675844387471</v>
+        <v>0.11206592272813662</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -919,7 +919,7 @@
       </c>
       <c r="B8" s="1">
         <f>SUM(B2:B7)</f>
-        <v>71768</v>
+        <v>73662</v>
       </c>
       <c r="C8" s="11">
         <f t="shared" si="0"/>
@@ -936,7 +936,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B13"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -964,7 +964,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2/$B$15</f>
-        <v>1.3113722198908938E-4</v>
+        <v>1.2470382840753212E-4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -976,7 +976,7 @@
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C15" si="0">B3/$B$15</f>
-        <v>2.360469995803609E-4</v>
+        <v>2.244668911335578E-4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -984,11 +984,11 @@
         <v>4</v>
       </c>
       <c r="B4" s="4">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" s="12">
         <f t="shared" si="0"/>
-        <v>6.5568610994544689E-4</v>
+        <v>6.4845990771916697E-4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -996,11 +996,11 @@
         <v>5</v>
       </c>
       <c r="B5" s="4">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" si="0"/>
-        <v>4.7996223248006715E-3</v>
+        <v>4.7886270108492331E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1008,11 +1008,11 @@
         <v>6</v>
       </c>
       <c r="B6" s="4">
-        <v>598</v>
+        <v>632</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" si="0"/>
-        <v>1.5684011749895092E-2</v>
+        <v>1.5762563910712058E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1020,11 +1020,11 @@
         <v>7</v>
       </c>
       <c r="B7" s="4">
-        <v>1789</v>
+        <v>1867</v>
       </c>
       <c r="C7" s="12">
         <f t="shared" si="0"/>
-        <v>4.6920898027696181E-2</v>
+        <v>4.6564409527372487E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1032,11 +1032,11 @@
         <v>8</v>
       </c>
       <c r="B8" s="4">
-        <v>4108</v>
+        <v>4320</v>
       </c>
       <c r="C8" s="12">
         <f t="shared" si="0"/>
-        <v>0.10774234158623584</v>
+        <v>0.10774410774410774</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1044,11 +1044,11 @@
         <v>9</v>
       </c>
       <c r="B9" s="4">
-        <v>3459</v>
+        <v>3659</v>
       </c>
       <c r="C9" s="12">
         <f t="shared" si="0"/>
-        <v>9.0720730172052039E-2</v>
+        <v>9.1258261628632001E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1056,11 +1056,11 @@
         <v>10</v>
       </c>
       <c r="B10" s="4">
-        <v>4463</v>
+        <v>4689</v>
       </c>
       <c r="C10" s="12">
         <f t="shared" si="0"/>
-        <v>0.11705308434746119</v>
+        <v>0.11694725028058361</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1068,11 +1068,11 @@
         <v>11</v>
       </c>
       <c r="B11" s="4">
-        <v>5061</v>
+        <v>5323</v>
       </c>
       <c r="C11" s="12">
         <f t="shared" si="0"/>
-        <v>0.13273709609735626</v>
+        <v>0.13275969572265869</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1080,11 +1080,11 @@
         <v>12</v>
       </c>
       <c r="B12" s="4">
-        <v>5072</v>
+        <v>5351</v>
       </c>
       <c r="C12" s="12">
         <f t="shared" si="0"/>
-        <v>0.13302559798573227</v>
+        <v>0.13345803716174087</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1092,11 +1092,11 @@
         <v>13</v>
       </c>
       <c r="B13" s="4">
-        <v>13356</v>
+        <v>14022</v>
       </c>
       <c r="C13" s="12">
         <f t="shared" si="0"/>
-        <v>0.35029374737725555</v>
+        <v>0.34971941638608306</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1117,7 +1117,7 @@
       </c>
       <c r="B15" s="8">
         <f>SUM(B2:B14)</f>
-        <v>38128</v>
+        <v>40095</v>
       </c>
       <c r="C15" s="15">
         <f t="shared" si="0"/>
@@ -1134,7 +1134,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1155,11 +1155,11 @@
         <v>16</v>
       </c>
       <c r="B2" s="7">
-        <v>16072</v>
+        <v>16854</v>
       </c>
       <c r="C2" s="12">
         <f>B2/$B$5</f>
-        <v>0.42152748636172893</v>
+        <v>0.42035166479610925</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1167,11 +1167,11 @@
         <v>17</v>
       </c>
       <c r="B3" s="7">
-        <v>22055</v>
+        <v>23240</v>
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C5" si="0">B3/$B$5</f>
-        <v>0.57844628619387328</v>
+        <v>0.57962339443820921</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="C4" s="12">
         <f t="shared" si="0"/>
-        <v>2.6227444397817876E-5</v>
+        <v>2.4940765681506424E-5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B5" s="1">
         <f>SUM(B2:B4)</f>
-        <v>38128</v>
+        <v>40095</v>
       </c>
       <c r="C5" s="16">
         <f t="shared" si="0"/>
@@ -1209,7 +1209,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1233,11 +1233,11 @@
         <v>23</v>
       </c>
       <c r="B2" s="10">
-        <v>735</v>
+        <v>800</v>
       </c>
       <c r="C2" s="12">
         <f>B2/$B$8</f>
-        <v>1.9277171632396138E-2</v>
+        <v>1.9952612545205139E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1245,11 +1245,11 @@
         <v>21</v>
       </c>
       <c r="B3" s="9">
-        <v>3629</v>
+        <v>3816</v>
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C8" si="0">B3/$B$8</f>
-        <v>9.5179395719681079E-2</v>
+        <v>9.5173961840628513E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1257,11 +1257,11 @@
         <v>22</v>
       </c>
       <c r="B4" s="10">
-        <v>17824</v>
+        <v>18648</v>
       </c>
       <c r="C4" s="12">
         <f t="shared" si="0"/>
-        <v>0.46747796894670585</v>
+        <v>0.46509539842873177</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1269,11 +1269,11 @@
         <v>25</v>
       </c>
       <c r="B5" s="10">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" si="0"/>
-        <v>5.2454888795635752E-3</v>
+        <v>5.2625015587978554E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1281,11 +1281,11 @@
         <v>20</v>
       </c>
       <c r="B6" s="4">
-        <v>15719</v>
+        <v>16598</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" si="0"/>
-        <v>0.41226919848929922</v>
+        <v>0.41396682878164359</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1293,11 +1293,11 @@
         <v>18</v>
       </c>
       <c r="B7" s="10">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="12">
         <f t="shared" si="0"/>
-        <v>5.5077633235417543E-4</v>
+        <v>5.4869684499314131E-4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1306,7 +1306,7 @@
       </c>
       <c r="B8" s="2">
         <f>SUM(B2:B7)</f>
-        <v>38128</v>
+        <v>40095</v>
       </c>
       <c r="C8" s="16">
         <f t="shared" si="0"/>

</xml_diff>